<commit_message>
B3: Added BOM for parts.
</commit_message>
<xml_diff>
--- a/Kicad/Trackball/Fabrication/Parts, Costs.xlsx
+++ b/Kicad/Trackball/Fabrication/Parts, Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak\Documents\GitHub\ThumbsUp-Trackball-v3\Kicad\Trackball\Fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A84EA1B-218C-47B7-ABB5-CB12DE520755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388EC5E3-4DB6-40C8-9E34-0BD2F4DD5D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{2F37D32B-8E94-44F1-AFD7-EC6CCC5D28C4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>6x  8x3mm Bumpons</t>
   </si>
@@ -141,7 +141,19 @@
     <t>Kailh Choc Key Cap</t>
   </si>
   <si>
-    <t>Price as sold at Etsy, less if ordered 20 sets from JLCPCB</t>
+    <t>Total without PCBs</t>
+  </si>
+  <si>
+    <t>M3 screws</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/dp/B07C72FBZ6</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Price as sold at Etsy, less if ordered 20 sets from JLCPCB  by yourself</t>
   </si>
 </sst>
 </file>
@@ -494,11 +506,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960A34CC-6418-4D7E-8CA8-2BAEC7E26B23}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -522,6 +532,9 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -558,7 +571,7 @@
         <v>6.7</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E19" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E20" si="0">C3*D3</f>
         <v>6.7</v>
       </c>
       <c r="F3" t="s">
@@ -891,29 +904,60 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <f xml:space="preserve"> 9.26*1.13/100</f>
+        <v>0.10463799999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41855199999999998</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D20" s="1">
         <v>60</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="F19" t="s">
-        <v>38</v>
+      <c r="F20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1">
+        <f>D24-D20</f>
+        <v>38.700538499999993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <f>SUM(D2:D22)</f>
-        <v>98.595900499999999</v>
+        <v>98.700538499999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>